<commit_message>
Deleted a row with lakshmi as email ID
</commit_message>
<xml_diff>
--- a/testData/Data.xlsx
+++ b/testData/Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Learning\OpenCartV121\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BB9CB84-6E50-4540-99DD-0D03567DA415}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99782DBE-66DF-4E8D-A324-842D3F2122B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FE44AFAA-F487-40C0-8B30-604EBAD62EDB}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{FE44AFAA-F487-40C0-8B30-604EBAD62EDB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>username</t>
   </si>
@@ -53,12 +53,6 @@
     <t>salim1234</t>
   </si>
   <si>
-    <t>lakshmi@yahoo.com</t>
-  </si>
-  <si>
-    <t>Lakkkk</t>
-  </si>
-  <si>
     <t>abc123@gmail.com</t>
   </si>
   <si>
@@ -66,9 +60,6 @@
   </si>
   <si>
     <t>Valid</t>
-  </si>
-  <si>
-    <t>Invalid</t>
   </si>
 </sst>
 </file>
@@ -474,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{050C98F0-6FA3-4865-AFF6-431862D95EE8}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -504,37 +495,25 @@
         <v>4</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{D4F36D5D-AC08-4B65-A2B3-6FAC36124DFD}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{156FACE9-D711-4DF3-8D85-10625DD1F63A}"/>
-    <hyperlink ref="A4" r:id="rId3" xr:uid="{1423CDDC-6C92-4F30-93F9-3327BD809B3D}"/>
-    <hyperlink ref="B4" r:id="rId4" xr:uid="{378E2F81-89BC-4FAD-A89E-0D4ED03538DD}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{1423CDDC-6C92-4F30-93F9-3327BD809B3D}"/>
+    <hyperlink ref="B3" r:id="rId3" xr:uid="{378E2F81-89BC-4FAD-A89E-0D4ED03538DD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>